<commit_message>
A star destroyer model added
</commit_message>
<xml_diff>
--- a/6028_Graph_1/D2D/W05/Attenuation.xlsx
+++ b/6028_Graph_1/D2D/W05/Attenuation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2021-2022\CODE\GDP2021_22\INFO6028\Lectures\W05.D01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2023-2024\GDP202324\6028_Graph_1\D2D\W05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{031F06AF-719A-4642-994A-71E34370C1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFE4D58-C197-412B-8B94-2A5030029571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D4E63752-553F-4195-9629-3BBB4B5CB0F6}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D4E63752-553F-4195-9629-3BBB4B5CB0F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Distance</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Brightness</t>
+  </si>
+  <si>
+    <t>Too big</t>
   </si>
 </sst>
 </file>
@@ -324,76 +327,76 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83333333333333326</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41666666666666663</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11904761904761901</c:v>
+                  <c:v>0.47619047619047605</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.9285714285714274E-2</c:v>
+                  <c:v>0.3571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9444444444444448E-2</c:v>
+                  <c:v>0.27777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>0.22222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5454545454545456E-2</c:v>
+                  <c:v>0.18181818181818182</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.7878787878787873E-2</c:v>
+                  <c:v>0.15151515151515149</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2051282051282048E-2</c:v>
+                  <c:v>0.12820512820512819</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7472527472527469E-2</c:v>
+                  <c:v>0.10989010989010987</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3809523809523808E-2</c:v>
+                  <c:v>9.5238095238095233E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.8382352941176468E-2</c:v>
+                  <c:v>7.3529411764705871E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6339869281045753E-2</c:v>
+                  <c:v>6.535947712418301E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.4619883040935675E-2</c:v>
+                  <c:v>5.8479532163742701E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.3157894736842105E-2</c:v>
+                  <c:v>5.2631578947368418E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.1904761904761904E-2</c:v>
+                  <c:v>4.7619047619047616E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0822510822510822E-2</c:v>
+                  <c:v>4.3290043290043288E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.8814229249011842E-3</c:v>
+                  <c:v>3.9525691699604737E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.057971014492754E-3</c:v>
+                  <c:v>3.6231884057971016E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.3333333333333315E-3</c:v>
+                  <c:v>3.3333333333333326E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.6923076923076927E-3</c:v>
+                  <c:v>3.0769230769230771E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,22 +1482,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2006BC04-CD87-41DC-9FC3-828377CB9051}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="5" width="8.7265625" style="1"/>
-    <col min="6" max="6" width="4.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1796875" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.77734375" style="1"/>
+    <col min="6" max="6" width="4.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -1527,19 +1530,19 @@
       </c>
       <c r="D2" s="1">
         <f>$M$3*A2</f>
-        <v>2.0000000000000003E-6</v>
+        <v>5.0000000000000008E-7</v>
       </c>
       <c r="E2" s="1">
         <f>$N$3*A2*A2</f>
-        <v>2.0000000000000005E-11</v>
+        <v>5.0000000000000013E-12</v>
       </c>
       <c r="G2" s="1">
         <f>E2+D2+C2</f>
-        <v>2.0000200000000005E-6</v>
+        <v>5.0000500000000012E-7</v>
       </c>
       <c r="H2" s="1">
         <f>1/G2</f>
-        <v>499995.00004999939</v>
+        <v>1999980.0001999976</v>
       </c>
       <c r="I2" s="4">
         <f>IF(H2&gt;1,1,H2)</f>
@@ -1558,7 +1561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <f>K3</f>
         <v>1</v>
@@ -1569,19 +1572,19 @@
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D27" si="1">$M$3*A3</f>
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E27" si="2">$N$3*A3*A3</f>
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G27" si="3">E3+D3+C3</f>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H27" si="4">1/G3</f>
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" ref="I3:I27" si="5">IF(H3&gt;1,1,H3)</f>
@@ -1594,15 +1597,21 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="N3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.05</v>
+      </c>
+      <c r="R3">
+        <v>0.5</v>
+      </c>
+      <c r="S3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <f>A3+$K$3</f>
+        <f t="shared" ref="A4:A27" si="6">A3+$K$3</f>
         <v>2</v>
       </c>
       <c r="C4" s="1">
@@ -1611,28 +1620,31 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="3"/>
-        <v>1.2000000000000002</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="4"/>
-        <v>0.83333333333333326</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="5"/>
-        <v>0.83333333333333326</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <f>A4+$K$3</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="C5" s="1">
@@ -1641,28 +1653,28 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>0.60000000000000009</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>1.8000000000000003</v>
+        <v>0.45000000000000007</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="3"/>
-        <v>2.4000000000000004</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="4"/>
-        <v>0.41666666666666663</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="5"/>
-        <v>0.41666666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <f>A5+$K$3</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="C6" s="1">
@@ -1671,28 +1683,28 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>3.2</v>
+        <v>0.8</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="5"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <f>A6+$K$3</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="C7" s="1">
@@ -1701,28 +1713,28 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1.25</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="5"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <f>A7+$K$3</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="C8" s="1">
@@ -1731,28 +1743,28 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>7.2000000000000011</v>
+        <v>1.8000000000000003</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="3"/>
-        <v>8.4000000000000021</v>
+        <v>2.1000000000000005</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="4"/>
-        <v>0.11904761904761901</v>
+        <v>0.47619047619047605</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="5"/>
-        <v>0.11904761904761901</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.47619047619047605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <f>A8+$K$3</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="C9" s="1">
@@ -1761,28 +1773,28 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>1.4000000000000001</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>9.8000000000000007</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="3"/>
-        <v>11.200000000000001</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="4"/>
-        <v>8.9285714285714274E-2</v>
+        <v>0.3571428571428571</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="5"/>
-        <v>8.9285714285714274E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.3571428571428571</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <f>A9+$K$3</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="C10" s="1">
@@ -1791,28 +1803,28 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>1.6</v>
+        <v>0.4</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>12.8</v>
+        <v>3.2</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="3"/>
-        <v>14.4</v>
+        <v>3.6</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="4"/>
-        <v>6.9444444444444448E-2</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="5"/>
-        <v>6.9444444444444448E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.27777777777777779</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <f>A10+$K$3</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="C11" s="1">
@@ -1821,28 +1833,28 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>1.8</v>
+        <v>0.45</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>16.2</v>
+        <v>4.05</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>4.5</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="4"/>
-        <v>5.5555555555555552E-2</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="5"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <f>A11+$K$3</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="C12" s="1">
@@ -1851,28 +1863,28 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>5.5</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="4"/>
-        <v>4.5454545454545456E-2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="5"/>
-        <v>4.5454545454545456E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <f>A12+$K$3</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="C13" s="1">
@@ -1881,28 +1893,28 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>24.200000000000003</v>
+        <v>6.0500000000000007</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="3"/>
-        <v>26.400000000000002</v>
+        <v>6.6000000000000005</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="4"/>
-        <v>3.7878787878787873E-2</v>
+        <v>0.15151515151515149</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="5"/>
-        <v>3.7878787878787873E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.15151515151515149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
-        <f>A13+$K$3</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="C14" s="1">
@@ -1911,28 +1923,28 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="2"/>
-        <v>28.800000000000004</v>
+        <v>7.2000000000000011</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="3"/>
-        <v>31.200000000000003</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="4"/>
-        <v>3.2051282051282048E-2</v>
+        <v>0.12820512820512819</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="5"/>
-        <v>3.2051282051282048E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.12820512820512819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <f>A14+$K$3</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="C15" s="1">
@@ -1941,28 +1953,28 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>2.6</v>
+        <v>0.65</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="2"/>
-        <v>33.800000000000004</v>
+        <v>8.4500000000000011</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="3"/>
-        <v>36.400000000000006</v>
+        <v>9.1000000000000014</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="4"/>
-        <v>2.7472527472527469E-2</v>
+        <v>0.10989010989010987</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="5"/>
-        <v>2.7472527472527469E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0.10989010989010987</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <f>A15+$K$3</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="C16" s="1">
@@ -1971,28 +1983,28 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>2.8000000000000003</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>39.200000000000003</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>10.5</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="4"/>
-        <v>2.3809523809523808E-2</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="5"/>
-        <v>2.3809523809523808E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>9.5238095238095233E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <f>A16+$K$3</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="C17" s="1">
@@ -2001,28 +2013,28 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>11.25</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="4"/>
-        <v>2.0833333333333332E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" si="5"/>
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <f>A17+$K$3</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="C18" s="1">
@@ -2031,28 +2043,28 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>3.2</v>
+        <v>0.8</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="2"/>
-        <v>51.2</v>
+        <v>12.8</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="3"/>
-        <v>54.400000000000006</v>
+        <v>13.600000000000001</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="4"/>
-        <v>1.8382352941176468E-2</v>
+        <v>7.3529411764705871E-2</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="5"/>
-        <v>1.8382352941176468E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>7.3529411764705871E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
-        <f>A18+$K$3</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="C19" s="1">
@@ -2061,28 +2073,28 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>3.4000000000000004</v>
+        <v>0.85000000000000009</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
-        <v>57.800000000000004</v>
+        <v>14.450000000000001</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>61.2</v>
+        <v>15.3</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="4"/>
-        <v>1.6339869281045753E-2</v>
+        <v>6.535947712418301E-2</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" si="5"/>
-        <v>1.6339869281045753E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>6.535947712418301E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
-        <f>A19+$K$3</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="C20" s="1">
@@ -2091,28 +2103,28 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
-        <v>3.6</v>
+        <v>0.9</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>64.8</v>
+        <v>16.2</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>68.399999999999991</v>
+        <v>17.099999999999998</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="4"/>
-        <v>1.4619883040935675E-2</v>
+        <v>5.8479532163742701E-2</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="5"/>
-        <v>1.4619883040935675E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>5.8479532163742701E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
-        <f>A20+$K$3</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="C21" s="1">
@@ -2121,28 +2133,28 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="1"/>
-        <v>3.8000000000000003</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
-        <v>72.2</v>
+        <v>18.05</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="4"/>
-        <v>1.3157894736842105E-2</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="5"/>
-        <v>1.3157894736842105E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>5.2631578947368418E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
-        <f>A21+$K$3</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="C22" s="1">
@@ -2151,28 +2163,28 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="4"/>
-        <v>1.1904761904761904E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="5"/>
-        <v>1.1904761904761904E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4.7619047619047616E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
-        <f>A22+$K$3</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="C23" s="1">
@@ -2181,28 +2193,28 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>4.2</v>
+        <v>1.05</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="2"/>
-        <v>88.2</v>
+        <v>22.05</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="3"/>
-        <v>92.4</v>
+        <v>23.1</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="4"/>
-        <v>1.0822510822510822E-2</v>
+        <v>4.3290043290043288E-2</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" si="5"/>
-        <v>1.0822510822510822E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>4.3290043290043288E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
-        <f>A23+$K$3</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="C24" s="1">
@@ -2211,28 +2223,28 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="2"/>
-        <v>96.800000000000011</v>
+        <v>24.200000000000003</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="3"/>
-        <v>101.20000000000002</v>
+        <v>25.300000000000004</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="4"/>
-        <v>9.8814229249011842E-3</v>
+        <v>3.9525691699604737E-2</v>
       </c>
       <c r="I24" s="4">
         <f t="shared" si="5"/>
-        <v>9.8814229249011842E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3.9525691699604737E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
-        <f>A24+$K$3</f>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="C25" s="1">
@@ -2241,28 +2253,28 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>4.6000000000000005</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="2"/>
-        <v>105.80000000000001</v>
+        <v>26.450000000000003</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="3"/>
-        <v>110.4</v>
+        <v>27.6</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="4"/>
-        <v>9.057971014492754E-3</v>
+        <v>3.6231884057971016E-2</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="5"/>
-        <v>9.057971014492754E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3.6231884057971016E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
-        <f>A25+$K$3</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="C26" s="1">
@@ -2271,28 +2283,28 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
-        <v>4.8000000000000007</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="2"/>
-        <v>115.20000000000002</v>
+        <v>28.800000000000004</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="3"/>
-        <v>120.00000000000001</v>
+        <v>30.000000000000004</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="4"/>
-        <v>8.3333333333333315E-3</v>
+        <v>3.3333333333333326E-2</v>
       </c>
       <c r="I26" s="4">
         <f t="shared" si="5"/>
-        <v>8.3333333333333315E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3.3333333333333326E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
-        <f>A26+$K$3</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="C27" s="1">
@@ -2301,23 +2313,23 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1.25</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>31.25</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>32.5</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="4"/>
-        <v>7.6923076923076927E-3</v>
+        <v>3.0769230769230771E-2</v>
       </c>
       <c r="I27" s="4">
         <f t="shared" si="5"/>
-        <v>7.6923076923076927E-3</v>
+        <v>3.0769230769230771E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting of sphere-triangle collision and response
</commit_message>
<xml_diff>
--- a/6028_Graph_1/D2D/W05/Attenuation.xlsx
+++ b/6028_Graph_1/D2D/W05/Attenuation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\00_GDP\2023-2024\GDP202324\6028_Graph_1\D2D\W05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFE4D58-C197-412B-8B94-2A5030029571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE45E74A-97DB-4526-BD7C-6B0C8FB95BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D4E63752-553F-4195-9629-3BBB4B5CB0F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D4E63752-553F-4195-9629-3BBB4B5CB0F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -330,73 +330,73 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.79365079365079361</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.59523809523809523</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.47619047619047616</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47619047619047605</c:v>
+                  <c:v>0.3968253968253968</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3571428571428571</c:v>
+                  <c:v>0.3401360544217687</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.27777777777777779</c:v>
+                  <c:v>0.29761904761904762</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22222222222222221</c:v>
+                  <c:v>0.26455026455026459</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.18181818181818182</c:v>
+                  <c:v>0.23809523809523808</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.15151515151515149</c:v>
+                  <c:v>0.21645021645021645</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.12820512820512819</c:v>
+                  <c:v>0.1984126984126984</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.10989010989010987</c:v>
+                  <c:v>0.18315018315018314</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>0.17006802721088435</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15873015873015872</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14880952380952381</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.14005602240896359</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1322751322751323</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12531328320802007</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.11904761904761904</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.11337868480725623</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.10822510822510822</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.10351966873706003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.9206349206349201E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>9.5238095238095233E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8.3333333333333329E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7.3529411764705871E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.535947712418301E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.8479532163742701E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.2631578947368418E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.7619047619047616E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.3290043290043288E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.9525691699604737E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.6231884057971016E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.3333333333333326E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.0769230769230771E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1485,7 +1485,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,19 +1530,19 @@
       </c>
       <c r="D2" s="1">
         <f>$M$3*A2</f>
-        <v>5.0000000000000008E-7</v>
+        <v>4.2000000000000004E-6</v>
       </c>
       <c r="E2" s="1">
         <f>$N$3*A2*A2</f>
-        <v>5.0000000000000013E-12</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
         <f>E2+D2+C2</f>
-        <v>5.0000500000000012E-7</v>
+        <v>4.2000000000000004E-6</v>
       </c>
       <c r="H2" s="1">
         <f>1/G2</f>
-        <v>1999980.0001999976</v>
+        <v>238095.23809523808</v>
       </c>
       <c r="I2" s="4">
         <f>IF(H2&gt;1,1,H2)</f>
@@ -1572,19 +1572,19 @@
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D27" si="1">$M$3*A3</f>
-        <v>0.05</v>
+        <v>0.42</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E27" si="2">$N$3*A3*A3</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G27" si="3">E3+D3+C3</f>
-        <v>0.1</v>
+        <v>0.42</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H27" si="4">1/G3</f>
-        <v>10</v>
+        <v>2.3809523809523809</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" ref="I3:I27" si="5">IF(H3&gt;1,1,H3)</f>
@@ -1597,10 +1597,10 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>0.05</v>
+        <v>0.42</v>
       </c>
       <c r="N3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0.5</v>
@@ -1620,19 +1620,19 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.84</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
+        <v>0.84</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="4"/>
-        <v>3.333333333333333</v>
+        <v>1.1904761904761905</v>
       </c>
       <c r="I4" s="4">
         <f t="shared" si="5"/>
@@ -1653,23 +1653,23 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>0.15000000000000002</v>
+        <v>1.26</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>0.45000000000000007</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="3"/>
-        <v>0.60000000000000009</v>
+        <v>1.26</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="4"/>
-        <v>1.6666666666666665</v>
+        <v>0.79365079365079361</v>
       </c>
       <c r="I5" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.79365079365079361</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -1683,23 +1683,23 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>1.68</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.68</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.59523809523809523</v>
       </c>
       <c r="I6" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.59523809523809523</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -1713,23 +1713,23 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>2.1</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="4"/>
-        <v>0.66666666666666663</v>
+        <v>0.47619047619047616</v>
       </c>
       <c r="I7" s="4">
         <f t="shared" si="5"/>
-        <v>0.66666666666666663</v>
+        <v>0.47619047619047616</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -1743,23 +1743,23 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <v>2.52</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>1.8000000000000003</v>
+        <v>0</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="3"/>
-        <v>2.1000000000000005</v>
+        <v>2.52</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="4"/>
-        <v>0.47619047619047605</v>
+        <v>0.3968253968253968</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="5"/>
-        <v>0.47619047619047605</v>
+        <v>0.3968253968253968</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -1773,23 +1773,23 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>0.35000000000000003</v>
+        <v>2.94</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>2.4500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="3"/>
-        <v>2.8000000000000003</v>
+        <v>2.94</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="4"/>
-        <v>0.3571428571428571</v>
+        <v>0.3401360544217687</v>
       </c>
       <c r="I9" s="4">
         <f t="shared" si="5"/>
-        <v>0.3571428571428571</v>
+        <v>0.3401360544217687</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1803,23 +1803,23 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>3.36</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="3"/>
-        <v>3.6</v>
+        <v>3.36</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="4"/>
-        <v>0.27777777777777779</v>
+        <v>0.29761904761904762</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="5"/>
-        <v>0.27777777777777779</v>
+        <v>0.29761904761904762</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1833,23 +1833,23 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>3.78</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>4.05</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>3.78</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="4"/>
-        <v>0.22222222222222221</v>
+        <v>0.26455026455026459</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="5"/>
-        <v>0.22222222222222221</v>
+        <v>0.26455026455026459</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1863,23 +1863,23 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>4.2</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="3"/>
-        <v>5.5</v>
+        <v>4.2</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="4"/>
-        <v>0.18181818181818182</v>
+        <v>0.23809523809523808</v>
       </c>
       <c r="I12" s="4">
         <f t="shared" si="5"/>
-        <v>0.18181818181818182</v>
+        <v>0.23809523809523808</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1893,23 +1893,23 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>0.55000000000000004</v>
+        <v>4.62</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="2"/>
-        <v>6.0500000000000007</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="3"/>
-        <v>6.6000000000000005</v>
+        <v>4.62</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="4"/>
-        <v>0.15151515151515149</v>
+        <v>0.21645021645021645</v>
       </c>
       <c r="I13" s="4">
         <f t="shared" si="5"/>
-        <v>0.15151515151515149</v>
+        <v>0.21645021645021645</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1923,23 +1923,23 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>0.60000000000000009</v>
+        <v>5.04</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="2"/>
-        <v>7.2000000000000011</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="3"/>
-        <v>7.8000000000000007</v>
+        <v>5.04</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="4"/>
-        <v>0.12820512820512819</v>
+        <v>0.1984126984126984</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="5"/>
-        <v>0.12820512820512819</v>
+        <v>0.1984126984126984</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -1953,23 +1953,23 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>0.65</v>
+        <v>5.46</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="2"/>
-        <v>8.4500000000000011</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="3"/>
-        <v>9.1000000000000014</v>
+        <v>5.46</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="4"/>
-        <v>0.10989010989010987</v>
+        <v>0.18315018315018314</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="5"/>
-        <v>0.10989010989010987</v>
+        <v>0.18315018315018314</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1983,23 +1983,23 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>0.70000000000000007</v>
+        <v>5.88</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="2"/>
-        <v>9.8000000000000007</v>
+        <v>0</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="3"/>
-        <v>10.5</v>
+        <v>5.88</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="4"/>
-        <v>9.5238095238095233E-2</v>
+        <v>0.17006802721088435</v>
       </c>
       <c r="I16" s="4">
         <f t="shared" si="5"/>
-        <v>9.5238095238095233E-2</v>
+        <v>0.17006802721088435</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -2013,23 +2013,23 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>6.3</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="2"/>
-        <v>11.25</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>6.3</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="4"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.15873015873015872</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" si="5"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.15873015873015872</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -2043,23 +2043,23 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>6.72</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="2"/>
-        <v>12.8</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="3"/>
-        <v>13.600000000000001</v>
+        <v>6.72</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="4"/>
-        <v>7.3529411764705871E-2</v>
+        <v>0.14880952380952381</v>
       </c>
       <c r="I18" s="4">
         <f t="shared" si="5"/>
-        <v>7.3529411764705871E-2</v>
+        <v>0.14880952380952381</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -2073,23 +2073,23 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>0.85000000000000009</v>
+        <v>7.14</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" si="2"/>
-        <v>14.450000000000001</v>
+        <v>0</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>15.3</v>
+        <v>7.14</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="4"/>
-        <v>6.535947712418301E-2</v>
+        <v>0.14005602240896359</v>
       </c>
       <c r="I19" s="4">
         <f t="shared" si="5"/>
-        <v>6.535947712418301E-2</v>
+        <v>0.14005602240896359</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -2103,23 +2103,23 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>7.56</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="2"/>
-        <v>16.2</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>17.099999999999998</v>
+        <v>7.56</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="4"/>
-        <v>5.8479532163742701E-2</v>
+        <v>0.1322751322751323</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" si="5"/>
-        <v>5.8479532163742701E-2</v>
+        <v>0.1322751322751323</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -2133,23 +2133,23 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="1"/>
-        <v>0.95000000000000007</v>
+        <v>7.9799999999999995</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="2"/>
-        <v>18.05</v>
+        <v>0</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>7.9799999999999995</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="4"/>
-        <v>5.2631578947368418E-2</v>
+        <v>0.12531328320802007</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="5"/>
-        <v>5.2631578947368418E-2</v>
+        <v>0.12531328320802007</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -2163,23 +2163,23 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>8.4</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>8.4</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="4"/>
-        <v>4.7619047619047616E-2</v>
+        <v>0.11904761904761904</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" si="5"/>
-        <v>4.7619047619047616E-2</v>
+        <v>0.11904761904761904</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -2193,23 +2193,23 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="1"/>
-        <v>1.05</v>
+        <v>8.82</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" si="2"/>
-        <v>22.05</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="3"/>
-        <v>23.1</v>
+        <v>8.82</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="4"/>
-        <v>4.3290043290043288E-2</v>
+        <v>0.11337868480725623</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" si="5"/>
-        <v>4.3290043290043288E-2</v>
+        <v>0.11337868480725623</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -2223,23 +2223,23 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>9.24</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" si="2"/>
-        <v>24.200000000000003</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="3"/>
-        <v>25.300000000000004</v>
+        <v>9.24</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="4"/>
-        <v>3.9525691699604737E-2</v>
+        <v>0.10822510822510822</v>
       </c>
       <c r="I24" s="4">
         <f t="shared" si="5"/>
-        <v>3.9525691699604737E-2</v>
+        <v>0.10822510822510822</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -2253,23 +2253,23 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="1"/>
-        <v>1.1500000000000001</v>
+        <v>9.66</v>
       </c>
       <c r="E25" s="1">
         <f t="shared" si="2"/>
-        <v>26.450000000000003</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="3"/>
-        <v>27.6</v>
+        <v>9.66</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="4"/>
-        <v>3.6231884057971016E-2</v>
+        <v>0.10351966873706003</v>
       </c>
       <c r="I25" s="4">
         <f t="shared" si="5"/>
-        <v>3.6231884057971016E-2</v>
+        <v>0.10351966873706003</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -2283,23 +2283,23 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
+        <v>10.08</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="2"/>
-        <v>28.800000000000004</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="3"/>
-        <v>30.000000000000004</v>
+        <v>10.08</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="4"/>
-        <v>3.3333333333333326E-2</v>
+        <v>9.9206349206349201E-2</v>
       </c>
       <c r="I26" s="4">
         <f t="shared" si="5"/>
-        <v>3.3333333333333326E-2</v>
+        <v>9.9206349206349201E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -2313,23 +2313,23 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>10.5</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="2"/>
-        <v>31.25</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="3"/>
-        <v>32.5</v>
+        <v>10.5</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="4"/>
-        <v>3.0769230769230771E-2</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="I27" s="4">
         <f t="shared" si="5"/>
-        <v>3.0769230769230771E-2</v>
+        <v>9.5238095238095233E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>